<commit_message>
Major code refactoring #422
</commit_message>
<xml_diff>
--- a/dsl/src/test/data/TabularActivityBuilderAndSplitDef.xlsx
+++ b/dsl/src/test/data/TabularActivityBuilderAndSplitDef.xlsx
@@ -3,16 +3,23 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{077996B9-7E5C-4252-AD10-1DEAC6B86FE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zsmyt\workspace\cristal-ise\dsl\src\test\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{206C26A9-DACE-4804-8226-1F2EB5374911}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14160" tabRatio="625" activeTab="1" xr2:uid="{A9C7762E-9BDD-441B-8C93-8BFC837C8F90}"/>
+    <workbookView xWindow="15" yWindow="0" windowWidth="25170" windowHeight="15300" tabRatio="625" activeTab="4" xr2:uid="{A9C7762E-9BDD-441B-8C93-8BFC837C8F90}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="5" r:id="rId1"/>
     <sheet name="StartWithAndSplit" sheetId="3" r:id="rId2"/>
+    <sheet name="SequenceWithAndSplit" sheetId="6" r:id="rId3"/>
+    <sheet name="NestedAndSplit" sheetId="7" r:id="rId4"/>
+    <sheet name="AndSplitWithLoop" sheetId="8" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="31">
   <si>
     <t>Description</t>
   </si>
@@ -85,6 +92,36 @@
   </si>
   <si>
     <t>Right</t>
+  </si>
+  <si>
+    <t>First</t>
+  </si>
+  <si>
+    <t>TestItem_Last:0</t>
+  </si>
+  <si>
+    <t>TestItem_First:0</t>
+  </si>
+  <si>
+    <t>Last</t>
+  </si>
+  <si>
+    <t>Loop</t>
+  </si>
+  <si>
+    <t>LoopEnd</t>
+  </si>
+  <si>
+    <t>Left1</t>
+  </si>
+  <si>
+    <t>Left2</t>
+  </si>
+  <si>
+    <t>Right1</t>
+  </si>
+  <si>
+    <t>Right2</t>
   </si>
 </sst>
 </file>
@@ -563,20 +600,20 @@
       <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.08984375" customWidth="1"/>
-    <col min="2" max="2" width="19.26953125" customWidth="1"/>
-    <col min="3" max="3" width="9.36328125" customWidth="1"/>
-    <col min="4" max="4" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>3</v>
       </c>
@@ -593,7 +630,7 @@
       <c r="H1" s="11"/>
       <c r="I1" s="11"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>4</v>
       </c>
@@ -622,7 +659,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>14</v>
       </c>
@@ -637,7 +674,7 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>16</v>
       </c>
@@ -650,7 +687,7 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
@@ -667,7 +704,7 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>17</v>
       </c>
@@ -680,7 +717,7 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>16</v>
       </c>
@@ -693,7 +730,7 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
@@ -710,7 +747,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>15</v>
       </c>
@@ -723,7 +760,7 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>15</v>
       </c>
@@ -750,25 +787,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ADC2A13-BBF2-4C2B-ADB3-E20C68234B9A}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.08984375" customWidth="1"/>
-    <col min="2" max="2" width="19.26953125" customWidth="1"/>
-    <col min="3" max="3" width="9.36328125" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>4</v>
       </c>
@@ -779,21 +816,21 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>14</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
@@ -804,21 +841,21 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
@@ -829,14 +866,412 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDB1BCE1-4DEA-4FE3-BBC4-6A0017F3920F}">
+  <dimension ref="A1:C14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.140625" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05AA6E25-2B85-4AA6-8D63-B033A198D98B}">
+  <dimension ref="A1:C15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.140625" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6439072-E111-4D98-923F-FAD35311A7B8}">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.140625" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
LoopWithAndSplit and AndSplitWithLoop #422
</commit_message>
<xml_diff>
--- a/dsl/src/test/data/TabularActivityBuilderAndSplitDef.xlsx
+++ b/dsl/src/test/data/TabularActivityBuilderAndSplitDef.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zsmyt\workspace\cristal-ise\dsl\src\test\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{206C26A9-DACE-4804-8226-1F2EB5374911}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{534910B0-5517-4E99-88D8-FE391C211160}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="0" windowWidth="25170" windowHeight="15300" tabRatio="625" activeTab="4" xr2:uid="{A9C7762E-9BDD-441B-8C93-8BFC837C8F90}"/>
+    <workbookView xWindow="30" yWindow="450" windowWidth="25170" windowHeight="15300" tabRatio="625" activeTab="4" xr2:uid="{A9C7762E-9BDD-441B-8C93-8BFC837C8F90}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="5" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="32">
   <si>
     <t>Description</t>
   </si>
@@ -122,6 +122,9 @@
   </si>
   <si>
     <t>Right2</t>
+  </si>
+  <si>
+    <t>LeftInLoop</t>
   </si>
 </sst>
 </file>
@@ -1183,17 +1186,17 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6439072-E111-4D98-923F-FAD35311A7B8}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.140625" customWidth="1"/>
     <col min="2" max="2" width="19.28515625" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1223,60 +1226,74 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="5" t="s">
         <v>25</v>
       </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
+        <v>7</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
build splits other than AdnSplit #422
</commit_message>
<xml_diff>
--- a/dsl/src/test/data/TabularActivityBuilderAndSplitDef.xlsx
+++ b/dsl/src/test/data/TabularActivityBuilderAndSplitDef.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zsmyt\workspace\cristal-ise\dsl\src\test\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C13B16C-09F9-4501-A174-00CF90BDA2CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A57CC6DF-42AA-4E83-ADD6-86510288137F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4620" yWindow="2655" windowWidth="18900" windowHeight="11115" tabRatio="625" firstSheet="5" activeTab="7" xr2:uid="{A9C7762E-9BDD-441B-8C93-8BFC837C8F90}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15540" tabRatio="625" firstSheet="3" activeTab="6" xr2:uid="{A9C7762E-9BDD-441B-8C93-8BFC837C8F90}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="5" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="41">
   <si>
     <t>Description</t>
   </si>
@@ -143,6 +143,18 @@
   </si>
   <si>
     <t>EndBlock</t>
+  </si>
+  <si>
+    <t>TestItem_Split:0</t>
+  </si>
+  <si>
+    <t>EndSplit</t>
+  </si>
+  <si>
+    <t>SplitLeft</t>
+  </si>
+  <si>
+    <t>SplitRight</t>
   </si>
 </sst>
 </file>
@@ -1326,7 +1338,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1430,8 +1442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BC606BA-C881-47BE-9871-A124E2FF7FD0}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1485,10 +1497,10 @@
         <v>7</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1510,10 +1522,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1525,7 +1537,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -1542,7 +1554,7 @@
         <v>7</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>20</v>
@@ -1574,7 +1586,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE177EBD-58BA-4889-B6F4-DD2F07353708}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>

</xml_diff>